<commit_message>
Added properties file and updated datas sheet
</commit_message>
<xml_diff>
--- a/ExcelSheet/MyExcel.xlsx
+++ b/ExcelSheet/MyExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahas\NewProjectTradeMe\ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928D5F43-8A96-4A34-ACD0-864124C807FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0536E7-8A3A-4EAE-8A12-A3BE7713B0DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Url</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Field</t>
   </si>
@@ -36,25 +33,35 @@
     <t>Value</t>
   </si>
   <si>
-    <t>https://www.tmsandbox.co.nz/</t>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Suburb_1</t>
+  </si>
+  <si>
+    <t>Suburb_2</t>
+  </si>
+  <si>
+    <t>Wellington</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>Kelburn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,16 +84,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -365,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -376,24 +380,45 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{2F4B59AC-1FE8-40C3-A40D-36A2E20DBC27}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>